<commit_message>
Sixth commit. Connecting logging to the project
</commit_message>
<xml_diff>
--- a/src/main/output/statistics.xlsx
+++ b/src/main/output/statistics.xlsx
@@ -29,28 +29,28 @@
     <t>Название университета</t>
   </si>
   <si>
+    <t>Медицина</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Московский Государственный Медицинский Университет; Тамбовский Университет Медицины; Самарский Медицинский Институт; </t>
+  </si>
+  <si>
+    <t>Лингвистика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Воронежский Литературно-Переводческий Университет; </t>
+  </si>
+  <si>
+    <t>Математика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Казанский Университет Вычислений; </t>
+  </si>
+  <si>
     <t>Физика</t>
   </si>
   <si>
     <t xml:space="preserve">Московский Выдуманный Университет; Московский Придуманный Институт; </t>
-  </si>
-  <si>
-    <t>Медицина</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Московский Государственный Медицинский Университет; Тамбовский Университет Медицины; Самарский Медицинский Институт; </t>
-  </si>
-  <si>
-    <t>Математика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Казанский Университет Вычислений; </t>
-  </si>
-  <si>
-    <t>Лингвистика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Воронежский Литературно-Переводческий Университет; </t>
   </si>
 </sst>
 </file>
@@ -134,13 +134,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>4.5</v>
+        <v>4.300000190734863</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>6</v>
@@ -151,13 +151,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>4.300000190734863</v>
+        <v>0.0</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>8</v>
@@ -185,13 +185,13 @@
         <v>11</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>0.0</v>
+        <v>4.5</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>12</v>

</xml_diff>

<commit_message>
The seventh commit. Working with XML, building the structure of an XML document, preparing for interaction with external systems, working with the file system
</commit_message>
<xml_diff>
--- a/src/main/output/statistics.xlsx
+++ b/src/main/output/statistics.xlsx
@@ -29,28 +29,28 @@
     <t>Название университета</t>
   </si>
   <si>
+    <t>Лингвистика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Воронежский Литературно-Переводческий Университет; </t>
+  </si>
+  <si>
+    <t>Физика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Московский Выдуманный Университет; Московский Придуманный Институт; </t>
+  </si>
+  <si>
     <t>Медицина</t>
   </si>
   <si>
     <t xml:space="preserve">Московский Государственный Медицинский Университет; Тамбовский Университет Медицины; Самарский Медицинский Институт; </t>
   </si>
   <si>
-    <t>Лингвистика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Воронежский Литературно-Переводческий Университет; </t>
-  </si>
-  <si>
     <t>Математика</t>
   </si>
   <si>
     <t xml:space="preserve">Казанский Университет Вычислений; </t>
-  </si>
-  <si>
-    <t>Физика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Московский Выдуманный Университет; Московский Придуманный Институт; </t>
   </si>
 </sst>
 </file>
@@ -134,13 +134,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>4.300000190734863</v>
+        <v>0.0</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>6</v>
@@ -151,13 +151,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>0.0</v>
+        <v>4.5</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>8</v>
@@ -168,13 +168,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>0.0</v>
+        <v>4.300000190734863</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>10</v>
@@ -185,13 +185,13 @@
         <v>11</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>4.5</v>
+        <v>0.0</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>12</v>

</xml_diff>